<commit_message>
Updating the counts with the combined files
</commit_message>
<xml_diff>
--- a/SVs_identification/results/counts_summary.xlsx
+++ b/SVs_identification/results/counts_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jj/breedmaps/SVs_identification/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CC8C0D-E095-9944-8C9D-D0F338CFFC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EEF7AA-FEFC-2647-B3B2-FCD6715DD4A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{C59E4963-226C-F644-A820-EC5271257A7A}"/>
+    <workbookView xWindow="9560" yWindow="500" windowWidth="19240" windowHeight="16320" activeTab="4" xr2:uid="{C59E4963-226C-F644-A820-EC5271257A7A}"/>
   </bookViews>
   <sheets>
     <sheet name="SV types and total counts" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="284">
   <si>
     <t>BTA131_S7_L001_R_SV</t>
   </si>
@@ -2744,8 +2744,8 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F354B53A-38AF-3248-B61B-783915AA008E}" name="Tabell8" displayName="Tabell8" ref="B2:L46" totalsRowCount="1">
-  <autoFilter ref="B2:L45" xr:uid="{87237158-0394-9242-84AC-FF771D458E21}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F354B53A-38AF-3248-B61B-783915AA008E}" name="Tabell8" displayName="Tabell8" ref="B2:L55" totalsRowCount="1">
+  <autoFilter ref="B2:L54" xr:uid="{87237158-0394-9242-84AC-FF771D458E21}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{08237B4C-D74E-6A4B-B688-5CF40DEA9F39}" name="FILE" totalsRowLabel="Summa"/>
     <tableColumn id="2" xr3:uid="{F2974413-9C5C-BE47-A8A6-85BC04FF76B9}" name="bos_taurus_structural_variations.gvf" totalsRowFunction="custom">
@@ -3427,8 +3427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B19324A-552D-B34B-9494-AC9A1A8ADE1D}">
   <dimension ref="A1:AD67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C57" sqref="A57:M67"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5949,51 +5949,51 @@
         <v>37</v>
       </c>
       <c r="B66" s="16">
-        <f>AVERAGE(B57:B65)</f>
+        <f t="shared" ref="B66:M66" si="4">AVERAGE(B57:B65)</f>
         <v>7842</v>
       </c>
       <c r="C66" s="16">
-        <f>AVERAGE(C57:C65)</f>
+        <f t="shared" si="4"/>
         <v>2359.6666666666665</v>
       </c>
       <c r="D66" s="16">
-        <f>AVERAGE(D57:D65)</f>
+        <f t="shared" si="4"/>
         <v>4191.7777777777774</v>
       </c>
       <c r="E66" s="16">
-        <f>AVERAGE(E57:E65)</f>
+        <f t="shared" si="4"/>
         <v>749.44444444444446</v>
       </c>
       <c r="F66" s="16">
-        <f>AVERAGE(F57:F65)</f>
+        <f t="shared" si="4"/>
         <v>968.44444444444446</v>
       </c>
       <c r="G66" s="16">
-        <f>AVERAGE(G57:G65)</f>
+        <f t="shared" si="4"/>
         <v>290.44444444444446</v>
       </c>
       <c r="H66" s="16">
-        <f>AVERAGE(H57:H65)</f>
+        <f t="shared" si="4"/>
         <v>1641.8888888888889</v>
       </c>
       <c r="I66" s="16">
-        <f>AVERAGE(I57:I65)</f>
+        <f t="shared" si="4"/>
         <v>1934.3333333333333</v>
       </c>
       <c r="J66" s="16">
-        <f>AVERAGE(J57:J65)</f>
+        <f t="shared" si="4"/>
         <v>26.777777777777779</v>
       </c>
       <c r="K66" s="16">
-        <f>AVERAGE(K57:K65)</f>
+        <f t="shared" si="4"/>
         <v>41.111111111111114</v>
       </c>
       <c r="L66" s="16">
-        <f>AVERAGE(L57:L65)</f>
+        <f t="shared" si="4"/>
         <v>289.33333333333331</v>
       </c>
       <c r="M66" s="16">
-        <f>AVERAGE(M57:M65)</f>
+        <f t="shared" si="4"/>
         <v>68.111111111111114</v>
       </c>
     </row>
@@ -6002,51 +6002,51 @@
         <v>36</v>
       </c>
       <c r="B67" s="14">
-        <f>SUM(B57:B65)</f>
+        <f t="shared" ref="B67:M67" si="5">SUM(B57:B65)</f>
         <v>70578</v>
       </c>
       <c r="C67" s="14">
-        <f>SUM(C57:C65)</f>
+        <f t="shared" si="5"/>
         <v>21237</v>
       </c>
       <c r="D67" s="14">
-        <f>SUM(D57:D65)</f>
+        <f t="shared" si="5"/>
         <v>37726</v>
       </c>
       <c r="E67" s="14">
-        <f>SUM(E57:E65)</f>
+        <f t="shared" si="5"/>
         <v>6745</v>
       </c>
       <c r="F67" s="14">
-        <f>SUM(F57:F65)</f>
+        <f t="shared" si="5"/>
         <v>8716</v>
       </c>
       <c r="G67" s="14">
-        <f>SUM(G57:G65)</f>
+        <f t="shared" si="5"/>
         <v>2614</v>
       </c>
       <c r="H67" s="14">
-        <f>SUM(H57:H65)</f>
+        <f t="shared" si="5"/>
         <v>14777</v>
       </c>
       <c r="I67" s="14">
-        <f>SUM(I57:I65)</f>
+        <f t="shared" si="5"/>
         <v>17409</v>
       </c>
       <c r="J67" s="14">
-        <f>SUM(J57:J65)</f>
+        <f t="shared" si="5"/>
         <v>241</v>
       </c>
       <c r="K67" s="14">
-        <f>SUM(K57:K65)</f>
+        <f t="shared" si="5"/>
         <v>370</v>
       </c>
       <c r="L67" s="14">
-        <f>SUM(L57:L65)</f>
+        <f t="shared" si="5"/>
         <v>2604</v>
       </c>
       <c r="M67" s="14">
-        <f>SUM(M57:M65)</f>
+        <f t="shared" si="5"/>
         <v>613</v>
       </c>
     </row>
@@ -6910,8 +6910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14AE3EEC-6BC4-2943-A696-7044327C8DC6}">
   <dimension ref="B1:AZ70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="R57" sqref="R57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12461,8 +12461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{457DAE9B-5C19-DE45-8744-FEE386C159C0}">
   <dimension ref="A1:AR45"/>
   <sheetViews>
-    <sheetView topLeftCell="D20" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15361,7 +15361,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="14" t="s">
+      <c r="A36" t="s">
         <v>191</v>
       </c>
       <c r="B36" t="s">
@@ -15399,7 +15399,7 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
+      <c r="A37" t="s">
         <v>182</v>
       </c>
       <c r="B37">
@@ -15439,7 +15439,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="15" t="s">
+      <c r="A38" t="s">
         <v>183</v>
       </c>
       <c r="B38">
@@ -15479,7 +15479,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
+      <c r="A39" t="s">
         <v>184</v>
       </c>
       <c r="B39">
@@ -15674,7 +15674,7 @@
         <v>928124</v>
       </c>
       <c r="L43">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(B43:J43)</f>
         <v>103124.88888888889</v>
       </c>
     </row>
@@ -15772,14 +15772,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B4B16D-1442-9743-A06A-2C1AE9E9A230}">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="C23" workbookViewId="0">
+      <selection activeCell="L55" sqref="L55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="37.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.5" bestFit="1" customWidth="1"/>
     <col min="4" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="9.1640625" bestFit="1" customWidth="1"/>
@@ -17374,131 +17375,446 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>36</v>
+        <v>254</v>
       </c>
       <c r="C46">
-        <f>SUM(Tabell8[bos_taurus_structural_variations.gvf])</f>
-        <v>188764</v>
+        <v>21155</v>
       </c>
       <c r="D46">
-        <f>SUM(Tabell8[estd223])</f>
-        <v>33557</v>
+        <v>3997</v>
       </c>
       <c r="E46">
-        <f>SUM(Tabell8[estd234])</f>
-        <v>15102</v>
+        <v>2146</v>
       </c>
       <c r="F46">
-        <f>SUM(Tabell8[nstd119])</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G46">
-        <f>SUM(Tabell8[nstd131])</f>
-        <v>14768</v>
+        <v>1697</v>
       </c>
       <c r="H46">
-        <f>SUM(Tabell8[nstd135])</f>
-        <v>1821</v>
+        <v>228</v>
       </c>
       <c r="I46">
-        <f>SUM(Tabell8[nstd56])</f>
-        <v>3945</v>
+        <v>524</v>
       </c>
       <c r="J46">
-        <f>SUM(Tabell8[nstd60])</f>
-        <v>9628</v>
+        <v>1278</v>
       </c>
       <c r="K46">
-        <f>SUM(Tabell8[nstd61])</f>
-        <v>4180</v>
+        <v>542</v>
       </c>
       <c r="L46">
-        <f>SUM(Tabell8[nstd69])</f>
-        <v>5367</v>
+        <v>657</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>153</v>
+        <v>247</v>
       </c>
       <c r="C47">
-        <f>AVERAGE(Tabell8[bos_taurus_structural_variations.gvf])</f>
-        <v>4389.8604651162786</v>
+        <v>22864</v>
       </c>
       <c r="D47">
-        <f>AVERAGE(Tabell8[estd223])</f>
-        <v>780.39534883720933</v>
+        <v>3350</v>
       </c>
       <c r="E47">
-        <f>AVERAGE(Tabell8[estd234])</f>
-        <v>351.2093023255814</v>
+        <v>1378</v>
       </c>
       <c r="F47">
-        <f>AVERAGE(Tabell8[nstd119])</f>
-        <v>6.9767441860465115E-2</v>
+        <v>1</v>
       </c>
       <c r="G47">
-        <f>AVERAGE(Tabell8[nstd131])</f>
-        <v>343.44186046511629</v>
+        <v>1327</v>
       </c>
       <c r="H47">
-        <f>AVERAGE(Tabell8[nstd135])</f>
-        <v>42.348837209302324</v>
+        <v>226</v>
       </c>
       <c r="I47">
-        <f>AVERAGE(Tabell8[nstd56])</f>
-        <v>91.744186046511629</v>
+        <v>374</v>
       </c>
       <c r="J47">
-        <f>AVERAGE(Tabell8[nstd60])</f>
-        <v>223.90697674418604</v>
+        <v>1096</v>
       </c>
       <c r="K47">
-        <f>AVERAGE(Tabell8[nstd61])</f>
-        <v>97.20930232558139</v>
+        <v>419</v>
       </c>
       <c r="L47">
-        <f>AVERAGE(Tabell8[nstd69])</f>
-        <v>124.81395348837209</v>
+        <v>516</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
+        <v>252</v>
+      </c>
+      <c r="C48">
+        <v>17657</v>
+      </c>
+      <c r="D48">
+        <v>2923</v>
+      </c>
+      <c r="E48">
+        <v>1122</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>856</v>
+      </c>
+      <c r="H48">
+        <v>144</v>
+      </c>
+      <c r="I48">
+        <v>233</v>
+      </c>
+      <c r="J48">
+        <v>850</v>
+      </c>
+      <c r="K48">
+        <v>378</v>
+      </c>
+      <c r="L48">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B49" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="C49">
+        <v>26989</v>
+      </c>
+      <c r="D49">
+        <v>4263</v>
+      </c>
+      <c r="E49">
+        <v>2292</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>3611</v>
+      </c>
+      <c r="H49">
+        <v>225</v>
+      </c>
+      <c r="I49">
+        <v>473</v>
+      </c>
+      <c r="J49">
+        <v>1143</v>
+      </c>
+      <c r="K49">
+        <v>559</v>
+      </c>
+      <c r="L49">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>246</v>
+      </c>
+      <c r="C50">
+        <v>15312</v>
+      </c>
+      <c r="D50">
+        <v>2246</v>
+      </c>
+      <c r="E50">
+        <v>794</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>1007</v>
+      </c>
+      <c r="H50">
+        <v>116</v>
+      </c>
+      <c r="I50">
+        <v>242</v>
+      </c>
+      <c r="J50">
+        <v>769</v>
+      </c>
+      <c r="K50">
+        <v>286</v>
+      </c>
+      <c r="L50">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>251</v>
+      </c>
+      <c r="C51">
+        <v>23417</v>
+      </c>
+      <c r="D51">
+        <v>3746</v>
+      </c>
+      <c r="E51">
+        <v>1666</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>1222</v>
+      </c>
+      <c r="H51">
+        <v>182</v>
+      </c>
+      <c r="I51">
+        <v>457</v>
+      </c>
+      <c r="J51">
+        <v>1070</v>
+      </c>
+      <c r="K51">
+        <v>486</v>
+      </c>
+      <c r="L51">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>248</v>
+      </c>
+      <c r="C52">
+        <v>23107</v>
+      </c>
+      <c r="D52">
+        <v>3740</v>
+      </c>
+      <c r="E52">
+        <v>1850</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>1746</v>
+      </c>
+      <c r="H52">
+        <v>215</v>
+      </c>
+      <c r="I52">
+        <v>466</v>
+      </c>
+      <c r="J52">
+        <v>1099</v>
+      </c>
+      <c r="K52">
+        <v>484</v>
+      </c>
+      <c r="L52">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B53" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="C53">
+        <v>15806</v>
+      </c>
+      <c r="D53">
+        <v>2716</v>
+      </c>
+      <c r="E53">
+        <v>1102</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>1391</v>
+      </c>
+      <c r="H53">
+        <v>153</v>
+      </c>
+      <c r="I53">
+        <v>300</v>
+      </c>
+      <c r="J53">
+        <v>725</v>
+      </c>
+      <c r="K53">
+        <v>333</v>
+      </c>
+      <c r="L53">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>249</v>
+      </c>
+      <c r="C54">
+        <v>19113</v>
+      </c>
+      <c r="D54">
+        <v>2880</v>
+      </c>
+      <c r="E54">
+        <v>1396</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>1266</v>
+      </c>
+      <c r="H54">
+        <v>220</v>
+      </c>
+      <c r="I54">
+        <v>406</v>
+      </c>
+      <c r="J54">
+        <v>910</v>
+      </c>
+      <c r="K54">
+        <v>459</v>
+      </c>
+      <c r="L54">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>36</v>
+      </c>
+      <c r="C55">
+        <f>SUM(Tabell8[bos_taurus_structural_variations.gvf])</f>
+        <v>374184</v>
+      </c>
+      <c r="D55">
+        <f>SUM(Tabell8[estd223])</f>
+        <v>63418</v>
+      </c>
+      <c r="E55">
+        <f>SUM(Tabell8[estd234])</f>
+        <v>28848</v>
+      </c>
+      <c r="F55">
+        <f>SUM(Tabell8[nstd119])</f>
+        <v>5</v>
+      </c>
+      <c r="G55">
+        <f>SUM(Tabell8[nstd131])</f>
+        <v>28891</v>
+      </c>
+      <c r="H55">
+        <f>SUM(Tabell8[nstd135])</f>
+        <v>3530</v>
+      </c>
+      <c r="I55">
+        <f>SUM(Tabell8[nstd56])</f>
+        <v>7420</v>
+      </c>
+      <c r="J55">
+        <f>SUM(Tabell8[nstd60])</f>
+        <v>18568</v>
+      </c>
+      <c r="K55">
+        <f>SUM(Tabell8[nstd61])</f>
+        <v>8126</v>
+      </c>
+      <c r="L55">
+        <f>SUM(Tabell8[nstd69])</f>
+        <v>10054</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>153</v>
+      </c>
+      <c r="C56">
+        <f>AVERAGE(Tabell8[bos_taurus_structural_variations.gvf])</f>
+        <v>7195.8461538461543</v>
+      </c>
+      <c r="D56">
+        <f>AVERAGE(Tabell8[estd223])</f>
+        <v>1219.5769230769231</v>
+      </c>
+      <c r="E56">
+        <f>AVERAGE(Tabell8[estd234])</f>
+        <v>554.76923076923072</v>
+      </c>
+      <c r="F56">
+        <f>AVERAGE(Tabell8[nstd119])</f>
+        <v>9.6153846153846159E-2</v>
+      </c>
+      <c r="G56">
+        <f>AVERAGE(Tabell8[nstd131])</f>
+        <v>555.59615384615381</v>
+      </c>
+      <c r="H56">
+        <f>AVERAGE(Tabell8[nstd135])</f>
+        <v>67.884615384615387</v>
+      </c>
+      <c r="I56">
+        <f>AVERAGE(Tabell8[nstd56])</f>
+        <v>142.69230769230768</v>
+      </c>
+      <c r="J56">
+        <f>AVERAGE(Tabell8[nstd60])</f>
+        <v>357.07692307692309</v>
+      </c>
+      <c r="K56">
+        <f>AVERAGE(Tabell8[nstd61])</f>
+        <v>156.26923076923077</v>
+      </c>
+      <c r="L56">
+        <f>AVERAGE(Tabell8[nstd69])</f>
+        <v>193.34615384615384</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
         <v>240</v>
       </c>
-      <c r="C48">
+      <c r="C57">
         <v>462845</v>
       </c>
-      <c r="D48">
+      <c r="D57">
         <v>31300</v>
       </c>
-      <c r="E48">
+      <c r="E57">
         <v>369238</v>
       </c>
-      <c r="F48">
+      <c r="F57">
         <v>3</v>
       </c>
-      <c r="G48">
+      <c r="G57">
         <v>240614</v>
       </c>
-      <c r="H48">
+      <c r="H57">
         <v>1736</v>
       </c>
-      <c r="I48">
+      <c r="I57">
         <v>6356</v>
       </c>
-      <c r="J48">
+      <c r="J57">
         <v>13233</v>
       </c>
-      <c r="K48">
+      <c r="K57">
         <v>4217</v>
       </c>
-      <c r="L48">
+      <c r="L57">
         <v>16899</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B51" s="13"/>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B60" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17513,7 +17829,7 @@
   <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E6:E7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>